<commit_message>
creation fonction retrouver building number
</commit_message>
<xml_diff>
--- a/Data/Premises.xlsx
+++ b/Data/Premises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre Beylard\Google Drive\Formation\CoursPython\Charges_immeuble\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B501E-069B-488A-BE72-4AC1DF8B1613}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7A4FC5-B0A5-4162-B6A5-422285085C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{80042073-1BC6-481A-A685-355CA24ED583}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Echoppe</t>
+  </si>
+  <si>
+    <t>Global Building</t>
   </si>
 </sst>
 </file>
@@ -593,17 +596,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B10F5B-5774-4EE3-871E-E06484DAAB39}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1806,6 +1809,76 @@
       </c>
       <c r="L33" s="5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>2</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>4</v>
+      </c>
+      <c r="B37" s="5">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>5</v>
+      </c>
+      <c r="B38" s="5">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>